<commit_message>
Selecting prices & ubications
</commit_message>
<xml_diff>
--- a/data_housing.xlsx
+++ b/data_housing.xlsx
@@ -19,148 +19,148 @@
     <t>Link</t>
   </si>
   <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2877020216-casa-de-4-recamaras-y-4-banos-una-en-planta-baja-con-acabados-de-lujo-_JM#position=1&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2019975937-casa-en-venta-de-3-recamaras-y-roof-en-zakia-queretaro-_JM#position=2&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2020052569-casa-campestre-en-venta-en-queretaro-_JM#position=3&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2020014713-casa-en-venta-en-condesa-juriquilla-con-recamara-en-pb-y-roof-top-_JM#position=4&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2021698087-residencia-de-autor-con-acabados-premium-altozano-_JM#position=5&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2021787853-vivir-con-altura-altozano-_JM#position=6&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2019975941-casa-en-venta-en-el-refugio-en-frente-de-amenidades-_JM#position=7&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2020039523-casa-en-venta-para-remodelar-centro-queretaro-_JM#position=8&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2020001495-viu-panorama-casa-de-autor-_JM#position=9&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2020398201-casa-en-venta-en-zibata-de-4-recamaras-y-roof-garden-ideal-_JM#position=10&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2020448879-casa-en-venta-en-altozano-de-2-recamaras-moderna-en-priv-_JM#position=11&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2020039557-casa-en-venta-3-recamaras-cada-una-con-su-bano-y-roof-garden-_JM#position=12&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2020052573-casa-de-arquitecto-en-venta-en-zakia-de-3-recamaras-_JM#position=13&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2020372783-casa-en-venta-en-zibata-con-4-habitaciones-y-cuarto-de-serv-_JM#position=14&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2020248527-casa-condominio-en-venta-santa-ines-lomas-el-campanario-_JM#position=15&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2020052563-casa-en-venta-en-el-refugio-queretaro-_JM#position=16&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2020078095-casa-en-venta-esquina-con-jardin-grande-en-queretaro-_JM#position=17&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2020474339-departamento-en-venta-en-central-park-amueblado-de-lujo-_JM#position=18&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2020398091-casa-en-venta-en-zibata-estilo-mexico-contemporanea-de-3-_JM#position=19&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2019988747-casa-en-venta-en-queretaro-en-privada-con-alberca-_JM#position=20&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2020064467-casa-lomas-del-campanario-_JM#position=21&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2021853869-residencia-con-acabados-premium-altozano-_JM#position=22&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2021698085-residencia-con-amplios-espacios-jurica-_JM#position=23&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2021800157-increible-casa-de-autor-zibata-_JM#position=24&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2021800155-doble-altura-amplio-jardin-la-vista-residencial-_JM#position=25&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2021762251-amplio-jardin-con-terraza-la-vista-residencial-_JM#position=26&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2885801136-la-vida-que-deseas-altozano-_JM#position=27&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2021762245-exclusividad-y-confort-zibata-_JM#position=28&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2021749071-vive-en-plenitud-lomas-del-campanario-norte-_JM#position=29&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2885801130-nuevas-emociones-altozano-_JM#position=30&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2021762239-una-vida-excepcional-altozano-_JM#position=31&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2021710635-residencia-con-acabados-premium-altozano-_JM#position=32&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2021710631-la-vida-que-deseas-la-vista-residencial-_JM#position=33&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2021774945-vive-en-armonia-canadas-del-arroyo-_JM#position=34&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2021774937-terraza-jardin-doble-altura-zibata-_JM#position=35&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2021762233-amplio-jardin-habitacion-en-planta-baja-zibata-_JM#position=36&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2885801124-diseno-unico-y-moderno-zibata-_JM#position=37&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2885801122-terraza-jardin-roof-garden-zibata-_JM#position=38&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2021762231-una-casa-de-altura-lomas-del-campanario-norte-_JM#position=39&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2885801116-conocela-y-enamorate-altozano-_JM#position=40&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2021736165-conocela-y-enamorate-lomas-del-campanario-norte-_JM#position=41&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2021800131-jardin-amplia-estancia-acceso-a-roof-colinas-de-juriquill-_JM#position=42&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2021736163-diseno-que-enamora-colinas-de-juriquilla-_JM#position=43&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2020435657-casa-en-venta-en-zibata-con-3-recamaras-dentro-de-condomin-_JM#position=44&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2021723537-canadas-del-arroyo-habitacion-planta-baja-_JM#position=45&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2020385347-casa-en-venta-en-santa-fe-juriquilla-dentro-de-privada-_JM#position=46&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2021710639-hasta-5-recamaras-roof-garden-milenio-lll-_JM#position=47&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
-  </si>
-  <si>
-    <t>https://casa.mercadolibre.com.mx/MLM-2021723553-distribuida-mayormente-en-una-planta-jurica-_JM#position=48&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62</t>
+    <t>https://casa.mercadolibre.com.mx/MLM-2021698087-residencia-de-autor-con-acabados-premium-altozano-_JM#position=1&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2021787853-vivir-con-altura-altozano-_JM#position=2&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2020248527-casa-condominio-en-venta-santa-ines-lomas-el-campanario-_JM#position=3&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2023177877-casa-en-venta-en-torre-de-piedra-gran-reserva-con-3-habitac-_JM#position=4&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2023037855-casa-en-venta-en-altozano-de-2-recamaras-moderna-en-priv-_JM#position=5&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2890670236-casa-en-venta-en-zibata-de-4-recamaras-y-roof-garden-ideal-_JM#position=6&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2023071019-casa-en-venta-en-zibata-con-4-habitaciones-y-cuarto-de-serv-_JM#position=7&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2023011467-casa-en-venta-en-zibata-estilo-mexico-contemporanea-de-3-_JM#position=8&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2889893070-4-habitaciones-amplio-jardin-la-condesa-juriquilla-_JM#position=9&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2889869734-4-habitaciones-amplio-jardin-la-condesa-juriquilla-_JM#position=10&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2021853869-residencia-con-acabados-premium-altozano-_JM#position=11&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2021698085-residencia-con-amplios-espacios-jurica-_JM#position=12&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2021800157-increible-casa-de-autor-zibata-_JM#position=13&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2021800155-doble-altura-amplio-jardin-la-vista-residencial-_JM#position=14&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2021762251-amplio-jardin-con-terraza-la-vista-residencial-_JM#position=15&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2885801136-la-vida-que-deseas-altozano-_JM#position=16&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2021762245-exclusividad-y-confort-zibata-_JM#position=17&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2021749071-vive-en-plenitud-lomas-del-campanario-norte-_JM#position=18&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2885801130-nuevas-emociones-altozano-_JM#position=19&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2021710635-residencia-con-acabados-premium-altozano-_JM#position=20&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2021762239-una-vida-excepcional-altozano-_JM#position=21&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2021774945-vive-en-armonia-canadas-del-arroyo-_JM#position=22&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2021710631-la-vida-que-deseas-la-vista-residencial-_JM#position=23&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2021774937-terraza-jardin-doble-altura-zibata-_JM#position=24&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2021762233-amplio-jardin-habitacion-en-planta-baja-zibata-_JM#position=25&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2885801124-diseno-unico-y-moderno-zibata-_JM#position=26&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2885801122-terraza-jardin-roof-garden-zibata-_JM#position=27&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2021762231-una-casa-de-altura-lomas-del-campanario-norte-_JM#position=28&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2885801116-conocela-y-enamorate-altozano-_JM#position=29&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2021736165-conocela-y-enamorate-lomas-del-campanario-norte-_JM#position=30&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2021800131-jardin-amplia-estancia-acceso-a-roof-colinas-de-juriquill-_JM#position=31&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2021736163-diseno-que-enamora-colinas-de-juriquilla-_JM#position=32&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2021723537-canadas-del-arroyo-habitacion-planta-baja-_JM#position=33&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2890670194-departamento-en-venta-en-central-park-amueblado-de-lujo-_JM#position=34&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2890740674-casa-en-venta-en-zibata-con-3-recamaras-dentro-de-condomin-_JM#position=35&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2021710639-hasta-5-recamaras-roof-garden-milenio-lll-_JM#position=36&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2890669990-casa-en-venta-en-santa-fe-juriquilla-dentro-de-privada-_JM#position=37&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2021723553-distribuida-mayormente-en-una-planta-jurica-_JM#position=38&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2021710637-acceso-a-roof-con-vista-pedregal-de-schoenstatt-_JM#position=39&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2885801128-casa-ensueno-juriquilla-_JM#position=40&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2021736177-habitacion-planta-baja-lomas-de-juriquilla-_JM#position=41&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2021736173-el-lujo-que-mereces-altozano-_JM#position=42&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2021800145-diseno-distintivo-zibata-_JM#position=43&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2021787865-tu-nuevo-hogar-residencial-el-refugio-_JM#position=44&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2890670252-casa-en-venta-en-altozano-dentro-de-condominio-con-alta-pl-_JM#position=45&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2890753436-exclusiva-casa-en-venta-en-altozano-dentro-de-condominio-c-_JM#position=46&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2021698081-iluminacion-y-amplitud-lomas-del-campanario-norte-_JM#position=47&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
+  </si>
+  <si>
+    <t>https://casa.mercadolibre.com.mx/MLM-2885801114-diseno-distintivo-la-espiga-_JM#position=48&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc</t>
   </si>
 </sst>
 </file>
@@ -928,54 +928,54 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" location="position=1&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B3" r:id="rId2" location="position=2&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B4" r:id="rId3" location="position=3&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B5" r:id="rId4" location="position=4&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B6" r:id="rId5" location="position=5&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B7" r:id="rId6" location="position=6&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B8" r:id="rId7" location="position=7&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B9" r:id="rId8" location="position=8&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B10" r:id="rId9" location="position=9&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B11" r:id="rId10" location="position=10&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B12" r:id="rId11" location="position=11&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B13" r:id="rId12" location="position=12&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B14" r:id="rId13" location="position=13&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B15" r:id="rId14" location="position=14&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B16" r:id="rId15" location="position=15&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B17" r:id="rId16" location="position=16&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B18" r:id="rId17" location="position=17&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B19" r:id="rId18" location="position=18&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B20" r:id="rId19" location="position=19&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B21" r:id="rId20" location="position=20&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B22" r:id="rId21" location="position=21&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B23" r:id="rId22" location="position=22&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B24" r:id="rId23" location="position=23&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B25" r:id="rId24" location="position=24&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B26" r:id="rId25" location="position=25&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B27" r:id="rId26" location="position=26&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B28" r:id="rId27" location="position=27&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B29" r:id="rId28" location="position=28&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B30" r:id="rId29" location="position=29&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B31" r:id="rId30" location="position=30&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B32" r:id="rId31" location="position=31&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B33" r:id="rId32" location="position=32&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B34" r:id="rId33" location="position=33&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B35" r:id="rId34" location="position=34&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B36" r:id="rId35" location="position=35&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B37" r:id="rId36" location="position=36&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B38" r:id="rId37" location="position=37&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B39" r:id="rId38" location="position=38&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B40" r:id="rId39" location="position=39&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B41" r:id="rId40" location="position=40&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B42" r:id="rId41" location="position=41&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B43" r:id="rId42" location="position=42&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B44" r:id="rId43" location="position=43&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B45" r:id="rId44" location="position=44&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B46" r:id="rId45" location="position=45&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B47" r:id="rId46" location="position=46&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B48" r:id="rId47" location="position=47&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
-    <hyperlink ref="B49" r:id="rId48" location="position=48&amp;search_layout=grid&amp;type=item&amp;tracking_id=b420d9c3-5257-45ef-a650-95972817ec62"/>
+    <hyperlink ref="B2" r:id="rId1" location="position=1&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B3" r:id="rId2" location="position=2&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B4" r:id="rId3" location="position=3&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B5" r:id="rId4" location="position=4&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B6" r:id="rId5" location="position=5&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B7" r:id="rId6" location="position=6&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B8" r:id="rId7" location="position=7&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B9" r:id="rId8" location="position=8&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B10" r:id="rId9" location="position=9&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B11" r:id="rId10" location="position=10&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B12" r:id="rId11" location="position=11&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B13" r:id="rId12" location="position=12&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B14" r:id="rId13" location="position=13&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B15" r:id="rId14" location="position=14&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B16" r:id="rId15" location="position=15&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B17" r:id="rId16" location="position=16&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B18" r:id="rId17" location="position=17&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B19" r:id="rId18" location="position=18&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B20" r:id="rId19" location="position=19&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B21" r:id="rId20" location="position=20&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B22" r:id="rId21" location="position=21&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B23" r:id="rId22" location="position=22&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B24" r:id="rId23" location="position=23&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B25" r:id="rId24" location="position=24&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B26" r:id="rId25" location="position=25&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B27" r:id="rId26" location="position=26&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B28" r:id="rId27" location="position=27&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B29" r:id="rId28" location="position=28&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B30" r:id="rId29" location="position=29&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B31" r:id="rId30" location="position=30&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B32" r:id="rId31" location="position=31&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B33" r:id="rId32" location="position=32&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B34" r:id="rId33" location="position=33&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B35" r:id="rId34" location="position=34&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B36" r:id="rId35" location="position=35&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B37" r:id="rId36" location="position=36&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B38" r:id="rId37" location="position=37&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B39" r:id="rId38" location="position=38&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B40" r:id="rId39" location="position=39&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B41" r:id="rId40" location="position=40&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B42" r:id="rId41" location="position=41&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B43" r:id="rId42" location="position=42&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B44" r:id="rId43" location="position=43&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B45" r:id="rId44" location="position=44&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B46" r:id="rId45" location="position=45&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B47" r:id="rId46" location="position=46&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B48" r:id="rId47" location="position=47&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
+    <hyperlink ref="B49" r:id="rId48" location="position=48&amp;search_layout=grid&amp;type=item&amp;tracking_id=fa943906-1423-4600-bb54-a94262abe0fc"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>